<commit_message>
14Dec2021 Selenium data driven Part1
</commit_message>
<xml_diff>
--- a/src/test/resources/AutomationDemoSIte.xlsx
+++ b/src/test/resources/AutomationDemoSIte.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\AugustBatchSelenium2021\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\SeleniumOctober_2021\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{2F3D61AC-072B-42F3-A178-2A1426BC425E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00534E7E-1C14-48BD-9596-70CF4A1D29ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="13276" windowWidth="20715" xWindow="-98" xr2:uid="{9F696F77-14B2-4A68-A1B1-E5EA60DF3651}" yWindow="-98"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{9F696F77-14B2-4A68-A1B1-E5EA60DF3651}"/>
   </bookViews>
   <sheets>
-    <sheet name="TestData" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet1" r:id="rId2" sheetId="2"/>
-    <sheet name="Sheet2" r:id="rId3" sheetId="3"/>
+    <sheet name="TestData" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">TestData!$A$1:$R$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestData!$A$1:$R$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="96">
   <si>
     <t>RunMode</t>
   </si>
@@ -327,16 +327,12 @@
   </si>
   <si>
     <t>validateDataDriven</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -386,25 +382,16 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -412,11 +399,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -433,10 +420,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -471,7 +458,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -523,7 +510,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -634,21 +621,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -665,7 +652,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -717,32 +704,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A98684-4136-4155-A927-F35C3B12F23B}">
-  <dimension ref="A1:T8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A98684-4136-4155-A927-F35C3B12F23B}">
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.9296875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.9296875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.59765625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="16.86328125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="1" max="1" width="10.9296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.9296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.59765625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.86328125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -856,15 +843,13 @@
       <c r="R2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="S2" t="s" s="15">
-        <v>96</v>
-      </c>
+      <c r="S2" s="6"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C3" t="s">
@@ -915,15 +900,13 @@
       <c r="R3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="S3" t="s" s="16">
-        <v>96</v>
-      </c>
+      <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C4" t="s">
@@ -974,13 +957,13 @@
       <c r="R4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="S4" s="5"/>
+      <c r="S4" s="3"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C5" t="s">
@@ -1031,15 +1014,13 @@
       <c r="R5" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="S5" t="s" s="17">
-        <v>96</v>
-      </c>
+      <c r="S5" s="8"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C6" t="s">
@@ -1090,15 +1071,13 @@
       <c r="R6" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="S6" t="s" s="18">
-        <v>96</v>
-      </c>
+      <c r="S6" s="9"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C7" t="s">
@@ -1149,13 +1128,13 @@
       <c r="R7" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="S7" s="8"/>
+      <c r="S7" s="4"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C8" t="s">
@@ -1206,61 +1185,59 @@
       <c r="R8" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="S8" t="s" s="19">
-        <v>96</v>
-      </c>
+      <c r="S8" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:R8" xr:uid="{88A98684-4136-4155-A927-F35C3B12F23B}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F2" xr:uid="{BD2F6444-EE39-428E-B42C-AC019C47E23F}"/>
-    <hyperlink r:id="rId2" ref="F3" xr:uid="{8B98C472-5E33-433A-8A34-13C87CDD75E1}"/>
-    <hyperlink r:id="rId3" ref="F4" xr:uid="{65BF28DE-B6E3-4786-8C97-8E34C70F9610}"/>
-    <hyperlink r:id="rId4" ref="F5" xr:uid="{E884CF7D-8EC6-44B5-9C78-29191CF8E72D}"/>
-    <hyperlink r:id="rId5" ref="F6" xr:uid="{25F205A4-0D5A-4232-B428-F2AFC044F4D5}"/>
-    <hyperlink r:id="rId6" ref="F7" xr:uid="{67FBDE13-938D-446A-8A63-35B55D9548C6}"/>
-    <hyperlink r:id="rId7" ref="F8" xr:uid="{6CFC3180-7416-48CB-AB9F-AB44912854CA}"/>
-    <hyperlink r:id="rId8" ref="Q2" xr:uid="{5CA725AA-0682-4EC9-B402-5A28CF6AB419}"/>
-    <hyperlink r:id="rId9" ref="Q3" xr:uid="{6209A8C4-BA2E-4362-97CD-E454F86DEBA2}"/>
-    <hyperlink r:id="rId10" ref="Q4" xr:uid="{44C3686F-D2A7-423B-A44D-471657BF32A8}"/>
-    <hyperlink r:id="rId11" ref="Q5" xr:uid="{DB62AEE6-9121-401A-A801-CDF76C06C1F4}"/>
-    <hyperlink r:id="rId12" ref="Q6" xr:uid="{07778A02-B08C-4DFE-BE77-011869797C1F}"/>
-    <hyperlink r:id="rId13" ref="Q7" xr:uid="{4E40552C-87A1-41E5-AD05-8FF72C69936B}"/>
-    <hyperlink r:id="rId14" ref="Q8" xr:uid="{47E8CBD7-1811-4553-BB48-9F10229CEF18}"/>
-    <hyperlink r:id="rId15" ref="R2" xr:uid="{C94FB2D9-DE65-49DF-AC12-07C0971DD409}"/>
-    <hyperlink r:id="rId16" ref="R3" xr:uid="{06E586DA-C9D0-44C0-8B84-C160A5EF7B04}"/>
-    <hyperlink r:id="rId17" ref="R4" xr:uid="{FA3B7ACF-3CE1-414D-A121-4816690D56AA}"/>
-    <hyperlink r:id="rId18" ref="R5" xr:uid="{1E2D8CA2-9006-424F-AB1D-610BE512C751}"/>
-    <hyperlink r:id="rId19" ref="R6" xr:uid="{DED1BB70-35F2-4D82-8C09-0C385B514029}"/>
-    <hyperlink r:id="rId20" ref="R7" xr:uid="{6711080A-BC56-4F23-9847-85FC74A422DF}"/>
-    <hyperlink r:id="rId21" ref="R8" xr:uid="{2164AB6D-0F96-4B7C-9B67-FB584364492B}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{BD2F6444-EE39-428E-B42C-AC019C47E23F}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{8B98C472-5E33-433A-8A34-13C87CDD75E1}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{65BF28DE-B6E3-4786-8C97-8E34C70F9610}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{E884CF7D-8EC6-44B5-9C78-29191CF8E72D}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{25F205A4-0D5A-4232-B428-F2AFC044F4D5}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{67FBDE13-938D-446A-8A63-35B55D9548C6}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{6CFC3180-7416-48CB-AB9F-AB44912854CA}"/>
+    <hyperlink ref="Q2" r:id="rId8" xr:uid="{5CA725AA-0682-4EC9-B402-5A28CF6AB419}"/>
+    <hyperlink ref="Q3" r:id="rId9" xr:uid="{6209A8C4-BA2E-4362-97CD-E454F86DEBA2}"/>
+    <hyperlink ref="Q4" r:id="rId10" xr:uid="{44C3686F-D2A7-423B-A44D-471657BF32A8}"/>
+    <hyperlink ref="Q5" r:id="rId11" xr:uid="{DB62AEE6-9121-401A-A801-CDF76C06C1F4}"/>
+    <hyperlink ref="Q6" r:id="rId12" xr:uid="{07778A02-B08C-4DFE-BE77-011869797C1F}"/>
+    <hyperlink ref="Q7" r:id="rId13" xr:uid="{4E40552C-87A1-41E5-AD05-8FF72C69936B}"/>
+    <hyperlink ref="Q8" r:id="rId14" xr:uid="{47E8CBD7-1811-4553-BB48-9F10229CEF18}"/>
+    <hyperlink ref="R2" r:id="rId15" xr:uid="{C94FB2D9-DE65-49DF-AC12-07C0971DD409}"/>
+    <hyperlink ref="R3" r:id="rId16" xr:uid="{06E586DA-C9D0-44C0-8B84-C160A5EF7B04}"/>
+    <hyperlink ref="R4" r:id="rId17" xr:uid="{FA3B7ACF-3CE1-414D-A121-4816690D56AA}"/>
+    <hyperlink ref="R5" r:id="rId18" xr:uid="{1E2D8CA2-9006-424F-AB1D-610BE512C751}"/>
+    <hyperlink ref="R6" r:id="rId19" xr:uid="{DED1BB70-35F2-4D82-8C09-0C385B514029}"/>
+    <hyperlink ref="R7" r:id="rId20" xr:uid="{6711080A-BC56-4F23-9847-85FC74A422DF}"/>
+    <hyperlink ref="R8" r:id="rId21" xr:uid="{2164AB6D-0F96-4B7C-9B67-FB584364492B}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId22"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B57123-EEDD-44D5-BA10-6ACA9AF90770}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B57123-EEDD-44D5-BA10-6ACA9AF90770}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD649DD5-9961-4A56-A72D-7AC48A9FF3A2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD649DD5-9961-4A56-A72D-7AC48A9FF3A2}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
16Dec2021 Selenium Data Driven part2"
</commit_message>
<xml_diff>
--- a/src/test/resources/AutomationDemoSIte.xlsx
+++ b/src/test/resources/AutomationDemoSIte.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\SeleniumOctober_2021\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00534E7E-1C14-48BD-9596-70CF4A1D29ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{00534E7E-1C14-48BD-9596-70CF4A1D29ED}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{9F696F77-14B2-4A68-A1B1-E5EA60DF3651}"/>
+    <workbookView windowHeight="13276" windowWidth="20715" xWindow="-98" xr2:uid="{9F696F77-14B2-4A68-A1B1-E5EA60DF3651}" yWindow="-98"/>
   </bookViews>
   <sheets>
-    <sheet name="TestData" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="TestData" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" r:id="rId2" sheetId="2"/>
+    <sheet name="Sheet2" r:id="rId3" sheetId="3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestData!$A$1:$R$8</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">TestData!$A$1:$R$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="97">
   <si>
     <t>RunMode</t>
   </si>
@@ -327,12 +327,16 @@
   </si>
   <si>
     <t>validateDataDriven</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -382,28 +386,29 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="12">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -420,10 +425,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -458,7 +463,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -510,7 +515,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -621,21 +626,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -652,7 +657,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -704,15 +709,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A98684-4136-4155-A927-F35C3B12F23B}">
-  <dimension ref="A1:S8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A98684-4136-4155-A927-F35C3B12F23B}">
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="Q11" sqref="Q11"/>
@@ -720,16 +725,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.9296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.9296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.59765625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.86328125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.9296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.9296875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.59765625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="16.86328125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row customFormat="1" r="1" s="1" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -843,7 +848,9 @@
       <c r="R2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="S2" s="6"/>
+      <c r="S2" t="s" s="11">
+        <v>96</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
@@ -1191,53 +1198,53 @@
   <autoFilter ref="A1:R8" xr:uid="{88A98684-4136-4155-A927-F35C3B12F23B}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{BD2F6444-EE39-428E-B42C-AC019C47E23F}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{8B98C472-5E33-433A-8A34-13C87CDD75E1}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{65BF28DE-B6E3-4786-8C97-8E34C70F9610}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{E884CF7D-8EC6-44B5-9C78-29191CF8E72D}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{25F205A4-0D5A-4232-B428-F2AFC044F4D5}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{67FBDE13-938D-446A-8A63-35B55D9548C6}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{6CFC3180-7416-48CB-AB9F-AB44912854CA}"/>
-    <hyperlink ref="Q2" r:id="rId8" xr:uid="{5CA725AA-0682-4EC9-B402-5A28CF6AB419}"/>
-    <hyperlink ref="Q3" r:id="rId9" xr:uid="{6209A8C4-BA2E-4362-97CD-E454F86DEBA2}"/>
-    <hyperlink ref="Q4" r:id="rId10" xr:uid="{44C3686F-D2A7-423B-A44D-471657BF32A8}"/>
-    <hyperlink ref="Q5" r:id="rId11" xr:uid="{DB62AEE6-9121-401A-A801-CDF76C06C1F4}"/>
-    <hyperlink ref="Q6" r:id="rId12" xr:uid="{07778A02-B08C-4DFE-BE77-011869797C1F}"/>
-    <hyperlink ref="Q7" r:id="rId13" xr:uid="{4E40552C-87A1-41E5-AD05-8FF72C69936B}"/>
-    <hyperlink ref="Q8" r:id="rId14" xr:uid="{47E8CBD7-1811-4553-BB48-9F10229CEF18}"/>
-    <hyperlink ref="R2" r:id="rId15" xr:uid="{C94FB2D9-DE65-49DF-AC12-07C0971DD409}"/>
-    <hyperlink ref="R3" r:id="rId16" xr:uid="{06E586DA-C9D0-44C0-8B84-C160A5EF7B04}"/>
-    <hyperlink ref="R4" r:id="rId17" xr:uid="{FA3B7ACF-3CE1-414D-A121-4816690D56AA}"/>
-    <hyperlink ref="R5" r:id="rId18" xr:uid="{1E2D8CA2-9006-424F-AB1D-610BE512C751}"/>
-    <hyperlink ref="R6" r:id="rId19" xr:uid="{DED1BB70-35F2-4D82-8C09-0C385B514029}"/>
-    <hyperlink ref="R7" r:id="rId20" xr:uid="{6711080A-BC56-4F23-9847-85FC74A422DF}"/>
-    <hyperlink ref="R8" r:id="rId21" xr:uid="{2164AB6D-0F96-4B7C-9B67-FB584364492B}"/>
+    <hyperlink r:id="rId1" ref="F2" xr:uid="{BD2F6444-EE39-428E-B42C-AC019C47E23F}"/>
+    <hyperlink r:id="rId2" ref="F3" xr:uid="{8B98C472-5E33-433A-8A34-13C87CDD75E1}"/>
+    <hyperlink r:id="rId3" ref="F4" xr:uid="{65BF28DE-B6E3-4786-8C97-8E34C70F9610}"/>
+    <hyperlink r:id="rId4" ref="F5" xr:uid="{E884CF7D-8EC6-44B5-9C78-29191CF8E72D}"/>
+    <hyperlink r:id="rId5" ref="F6" xr:uid="{25F205A4-0D5A-4232-B428-F2AFC044F4D5}"/>
+    <hyperlink r:id="rId6" ref="F7" xr:uid="{67FBDE13-938D-446A-8A63-35B55D9548C6}"/>
+    <hyperlink r:id="rId7" ref="F8" xr:uid="{6CFC3180-7416-48CB-AB9F-AB44912854CA}"/>
+    <hyperlink r:id="rId8" ref="Q2" xr:uid="{5CA725AA-0682-4EC9-B402-5A28CF6AB419}"/>
+    <hyperlink r:id="rId9" ref="Q3" xr:uid="{6209A8C4-BA2E-4362-97CD-E454F86DEBA2}"/>
+    <hyperlink r:id="rId10" ref="Q4" xr:uid="{44C3686F-D2A7-423B-A44D-471657BF32A8}"/>
+    <hyperlink r:id="rId11" ref="Q5" xr:uid="{DB62AEE6-9121-401A-A801-CDF76C06C1F4}"/>
+    <hyperlink r:id="rId12" ref="Q6" xr:uid="{07778A02-B08C-4DFE-BE77-011869797C1F}"/>
+    <hyperlink r:id="rId13" ref="Q7" xr:uid="{4E40552C-87A1-41E5-AD05-8FF72C69936B}"/>
+    <hyperlink r:id="rId14" ref="Q8" xr:uid="{47E8CBD7-1811-4553-BB48-9F10229CEF18}"/>
+    <hyperlink r:id="rId15" ref="R2" xr:uid="{C94FB2D9-DE65-49DF-AC12-07C0971DD409}"/>
+    <hyperlink r:id="rId16" ref="R3" xr:uid="{06E586DA-C9D0-44C0-8B84-C160A5EF7B04}"/>
+    <hyperlink r:id="rId17" ref="R4" xr:uid="{FA3B7ACF-3CE1-414D-A121-4816690D56AA}"/>
+    <hyperlink r:id="rId18" ref="R5" xr:uid="{1E2D8CA2-9006-424F-AB1D-610BE512C751}"/>
+    <hyperlink r:id="rId19" ref="R6" xr:uid="{DED1BB70-35F2-4D82-8C09-0C385B514029}"/>
+    <hyperlink r:id="rId20" ref="R7" xr:uid="{6711080A-BC56-4F23-9847-85FC74A422DF}"/>
+    <hyperlink r:id="rId21" ref="R8" xr:uid="{2164AB6D-0F96-4B7C-9B67-FB584364492B}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId22"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B57123-EEDD-44D5-BA10-6ACA9AF90770}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B57123-EEDD-44D5-BA10-6ACA9AF90770}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD649DD5-9961-4A56-A72D-7AC48A9FF3A2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD649DD5-9961-4A56-A72D-7AC48A9FF3A2}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
17Dec2021 Selenium DataDriven Part4
</commit_message>
<xml_diff>
--- a/src/test/resources/AutomationDemoSIte.xlsx
+++ b/src/test/resources/AutomationDemoSIte.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="97">
   <si>
     <t>RunMode</t>
   </si>
@@ -389,7 +389,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
@@ -401,6 +401,10 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
@@ -848,7 +852,7 @@
       <c r="R2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="S2" t="s" s="11">
+      <c r="S2" t="s" s="13">
         <v>96</v>
       </c>
     </row>
@@ -907,7 +911,9 @@
       <c r="R3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="S3" s="7"/>
+      <c r="S3" t="s" s="14">
+        <v>96</v>
+      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
@@ -1021,7 +1027,9 @@
       <c r="R5" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="S5" s="8"/>
+      <c r="S5" t="s" s="15">
+        <v>96</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A6" t="s">

</xml_diff>